<commit_message>
update from new pc
</commit_message>
<xml_diff>
--- a/data/3.meta_data/basic_info/25_01_31_basic_info.xlsx
+++ b/data/3.meta_data/basic_info/25_01_31_basic_info.xlsx
@@ -432,7 +432,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>review_topic_main</t>
+          <t>review_topics</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>bf_frame</t>
+          <t>trait_frame</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -707,12 +707,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>skilltraitdifferences; incrementalvalidity; academicachievement;</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; skilltraitdifferences; incrementalvalidity; otherreport</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>individual_differences</t>
+          <t>ses; gender; age</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>academicachievement; learningdisabilities</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1187,12 +1187,12 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>academicachievement; learningdisabilities; disabilities</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1314,12 +1314,12 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>nomoligicalnet</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>nomoligicalnet</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; shortversions</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1671,12 +1671,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1808,12 +1808,12 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1945,12 +1945,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>academicachievement; incrementalvalidity; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>change</t>
+          <t>normativechange; age; gender</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -2333,12 +2333,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>academicachievement; incrementalvalidity; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -2470,12 +2470,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>prosociality</t>
+          <t>volunteering</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2602,12 +2602,12 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>academicachievement; incrementalvalidity; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2734,12 +2734,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; behavioralassessment</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2866,12 +2866,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2984,12 +2984,12 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -3110,12 +3110,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; nomologicalnet; languageadaptation</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -3241,12 +3241,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -3363,12 +3363,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -3485,12 +3485,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -3617,12 +3617,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -3749,12 +3749,12 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -3881,12 +3881,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -4013,12 +4013,12 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>measurement</t>
+          <t>skillassessment; selfreport; otherreport; incrementalvalidity; nomologicalnet; skilltraitdifferences</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>meta</t>
+          <t>both</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>theoretical</t>
+          <t>theorydevelopment</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">

</xml_diff>